<commit_message>
Bold fonts, fill_and_border method to handle filling and border application
</commit_message>
<xml_diff>
--- a/workout_plan_new.xlsx
+++ b/workout_plan_new.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,8 +25,11 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -35,26 +38,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0095AB36"/>
-        <bgColor rgb="0095AB36"/>
+        <fgColor rgb="00FFCDAD"/>
+        <bgColor rgb="00FFCDAD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00A3BA3B"/>
-        <bgColor rgb="00A3BA3B"/>
+        <fgColor rgb="00FFC099"/>
+        <bgColor rgb="00FFC099"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00B3C45A"/>
-        <bgColor rgb="00B3C45A"/>
+        <fgColor rgb="00FFB485"/>
+        <bgColor rgb="00FFB485"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ADC445"/>
-        <bgColor rgb="00ADC445"/>
+        <fgColor rgb="00FFA770"/>
+        <bgColor rgb="00FFA770"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF9A5C"/>
+        <bgColor rgb="00FF9A5C"/>
       </patternFill>
     </fill>
   </fills>
@@ -142,19 +151,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -849,49 +858,49 @@
       <c r="D6" s="8" t="n"/>
       <c r="E6" s="9" t="inlineStr">
         <is>
-          <t>Set</t>
+          <t>Reps</t>
         </is>
       </c>
       <c r="F6" s="9" t="inlineStr">
         <is>
-          <t>Rep</t>
+          <t>Sets</t>
         </is>
       </c>
       <c r="G6" s="9" t="inlineStr">
         <is>
-          <t>Load</t>
+          <t>%1RM</t>
         </is>
       </c>
       <c r="H6" s="8" t="n"/>
       <c r="I6" s="9" t="inlineStr">
         <is>
-          <t>Set</t>
+          <t>Reps</t>
         </is>
       </c>
       <c r="J6" s="9" t="inlineStr">
         <is>
-          <t>Rep</t>
+          <t>Sets</t>
         </is>
       </c>
       <c r="K6" s="9" t="inlineStr">
         <is>
-          <t>Load</t>
+          <t>%1RM</t>
         </is>
       </c>
       <c r="L6" s="8" t="n"/>
       <c r="M6" s="9" t="inlineStr">
         <is>
-          <t>Set</t>
+          <t>Reps</t>
         </is>
       </c>
       <c r="N6" s="9" t="inlineStr">
         <is>
-          <t>Rep</t>
+          <t>Sets</t>
         </is>
       </c>
       <c r="O6" s="9" t="inlineStr">
         <is>
-          <t>Load</t>
+          <t>%1RM</t>
         </is>
       </c>
       <c r="P6" s="7" t="n"/>
@@ -900,49 +909,49 @@
       <c r="V6" s="8" t="n"/>
       <c r="W6" s="9" t="inlineStr">
         <is>
-          <t>Set</t>
+          <t>Reps</t>
         </is>
       </c>
       <c r="X6" s="9" t="inlineStr">
         <is>
-          <t>Rep</t>
+          <t>Sets</t>
         </is>
       </c>
       <c r="Y6" s="9" t="inlineStr">
         <is>
-          <t>Load</t>
+          <t>%1RM</t>
         </is>
       </c>
       <c r="Z6" s="8" t="n"/>
       <c r="AA6" s="9" t="inlineStr">
         <is>
-          <t>Set</t>
+          <t>Reps</t>
         </is>
       </c>
       <c r="AB6" s="9" t="inlineStr">
         <is>
-          <t>Rep</t>
+          <t>Sets</t>
         </is>
       </c>
       <c r="AC6" s="9" t="inlineStr">
         <is>
-          <t>Load</t>
+          <t>%1RM</t>
         </is>
       </c>
       <c r="AD6" s="8" t="n"/>
       <c r="AE6" s="9" t="inlineStr">
         <is>
-          <t>Set</t>
+          <t>Reps</t>
         </is>
       </c>
       <c r="AF6" s="9" t="inlineStr">
         <is>
-          <t>Rep</t>
+          <t>Sets</t>
         </is>
       </c>
       <c r="AG6" s="9" t="inlineStr">
         <is>
-          <t>Load</t>
+          <t>%1RM</t>
         </is>
       </c>
       <c r="AH6" s="7" t="n"/>
@@ -951,49 +960,49 @@
       <c r="AN6" s="8" t="n"/>
       <c r="AO6" s="9" t="inlineStr">
         <is>
-          <t>Set</t>
+          <t>Reps</t>
         </is>
       </c>
       <c r="AP6" s="9" t="inlineStr">
         <is>
-          <t>Rep</t>
+          <t>Sets</t>
         </is>
       </c>
       <c r="AQ6" s="9" t="inlineStr">
         <is>
-          <t>Load</t>
+          <t>%1RM</t>
         </is>
       </c>
       <c r="AR6" s="8" t="n"/>
       <c r="AS6" s="9" t="inlineStr">
         <is>
-          <t>Set</t>
+          <t>Reps</t>
         </is>
       </c>
       <c r="AT6" s="9" t="inlineStr">
         <is>
-          <t>Rep</t>
+          <t>Sets</t>
         </is>
       </c>
       <c r="AU6" s="9" t="inlineStr">
         <is>
-          <t>Load</t>
+          <t>%1RM</t>
         </is>
       </c>
       <c r="AV6" s="8" t="n"/>
       <c r="AW6" s="9" t="inlineStr">
         <is>
-          <t>Set</t>
+          <t>Reps</t>
         </is>
       </c>
       <c r="AX6" s="9" t="inlineStr">
         <is>
-          <t>Rep</t>
+          <t>Sets</t>
         </is>
       </c>
       <c r="AY6" s="9" t="inlineStr">
         <is>
-          <t>Load</t>
+          <t>%1RM</t>
         </is>
       </c>
       <c r="AZ6" s="7" t="n"/>
@@ -1002,49 +1011,49 @@
       <c r="BF6" s="8" t="n"/>
       <c r="BG6" s="9" t="inlineStr">
         <is>
-          <t>Set</t>
+          <t>Reps</t>
         </is>
       </c>
       <c r="BH6" s="9" t="inlineStr">
         <is>
-          <t>Rep</t>
+          <t>Sets</t>
         </is>
       </c>
       <c r="BI6" s="9" t="inlineStr">
         <is>
-          <t>Load</t>
+          <t>%1RM</t>
         </is>
       </c>
       <c r="BJ6" s="8" t="n"/>
       <c r="BK6" s="9" t="inlineStr">
         <is>
-          <t>Set</t>
+          <t>Reps</t>
         </is>
       </c>
       <c r="BL6" s="9" t="inlineStr">
         <is>
-          <t>Rep</t>
+          <t>Sets</t>
         </is>
       </c>
       <c r="BM6" s="9" t="inlineStr">
         <is>
-          <t>Load</t>
+          <t>%1RM</t>
         </is>
       </c>
       <c r="BN6" s="8" t="n"/>
       <c r="BO6" s="9" t="inlineStr">
         <is>
-          <t>Set</t>
+          <t>Reps</t>
         </is>
       </c>
       <c r="BP6" s="9" t="inlineStr">
         <is>
-          <t>Rep</t>
+          <t>Sets</t>
         </is>
       </c>
       <c r="BQ6" s="9" t="inlineStr">
         <is>
-          <t>Load</t>
+          <t>%1RM</t>
         </is>
       </c>
       <c r="BR6" s="7" t="n"/>
@@ -1119,17 +1128,17 @@
         </is>
       </c>
       <c r="D8" s="8" t="n"/>
-      <c r="E8" s="10" t="n"/>
-      <c r="F8" s="10" t="n"/>
-      <c r="G8" s="10" t="n"/>
+      <c r="E8" s="11" t="n"/>
+      <c r="F8" s="11" t="n"/>
+      <c r="G8" s="11" t="n"/>
       <c r="H8" s="8" t="n"/>
-      <c r="I8" s="10" t="n"/>
-      <c r="J8" s="10" t="n"/>
-      <c r="K8" s="10" t="n"/>
+      <c r="I8" s="11" t="n"/>
+      <c r="J8" s="11" t="n"/>
+      <c r="K8" s="11" t="n"/>
       <c r="L8" s="8" t="n"/>
-      <c r="M8" s="10" t="n"/>
-      <c r="N8" s="10" t="n"/>
-      <c r="O8" s="10" t="n"/>
+      <c r="M8" s="11" t="n"/>
+      <c r="N8" s="11" t="n"/>
+      <c r="O8" s="11" t="n"/>
       <c r="P8" s="7" t="n"/>
       <c r="T8" s="4" t="n"/>
       <c r="U8" s="10" t="inlineStr">
@@ -1138,17 +1147,17 @@
         </is>
       </c>
       <c r="V8" s="8" t="n"/>
-      <c r="W8" s="10" t="n"/>
-      <c r="X8" s="10" t="n"/>
-      <c r="Y8" s="10" t="n"/>
+      <c r="W8" s="11" t="n"/>
+      <c r="X8" s="11" t="n"/>
+      <c r="Y8" s="11" t="n"/>
       <c r="Z8" s="8" t="n"/>
-      <c r="AA8" s="10" t="n"/>
-      <c r="AB8" s="10" t="n"/>
-      <c r="AC8" s="10" t="n"/>
+      <c r="AA8" s="11" t="n"/>
+      <c r="AB8" s="11" t="n"/>
+      <c r="AC8" s="11" t="n"/>
       <c r="AD8" s="8" t="n"/>
-      <c r="AE8" s="10" t="n"/>
-      <c r="AF8" s="10" t="n"/>
-      <c r="AG8" s="10" t="n"/>
+      <c r="AE8" s="11" t="n"/>
+      <c r="AF8" s="11" t="n"/>
+      <c r="AG8" s="11" t="n"/>
       <c r="AH8" s="7" t="n"/>
       <c r="AL8" s="4" t="n"/>
       <c r="AM8" s="10" t="inlineStr">
@@ -1157,17 +1166,17 @@
         </is>
       </c>
       <c r="AN8" s="8" t="n"/>
-      <c r="AO8" s="10" t="n"/>
-      <c r="AP8" s="10" t="n"/>
-      <c r="AQ8" s="10" t="n"/>
+      <c r="AO8" s="11" t="n"/>
+      <c r="AP8" s="11" t="n"/>
+      <c r="AQ8" s="11" t="n"/>
       <c r="AR8" s="8" t="n"/>
-      <c r="AS8" s="10" t="n"/>
-      <c r="AT8" s="10" t="n"/>
-      <c r="AU8" s="10" t="n"/>
+      <c r="AS8" s="11" t="n"/>
+      <c r="AT8" s="11" t="n"/>
+      <c r="AU8" s="11" t="n"/>
       <c r="AV8" s="8" t="n"/>
-      <c r="AW8" s="10" t="n"/>
-      <c r="AX8" s="10" t="n"/>
-      <c r="AY8" s="10" t="n"/>
+      <c r="AW8" s="11" t="n"/>
+      <c r="AX8" s="11" t="n"/>
+      <c r="AY8" s="11" t="n"/>
       <c r="AZ8" s="7" t="n"/>
       <c r="BD8" s="4" t="n"/>
       <c r="BE8" s="10" t="inlineStr">
@@ -1176,17 +1185,17 @@
         </is>
       </c>
       <c r="BF8" s="8" t="n"/>
-      <c r="BG8" s="10" t="n"/>
-      <c r="BH8" s="10" t="n"/>
-      <c r="BI8" s="10" t="n"/>
+      <c r="BG8" s="11" t="n"/>
+      <c r="BH8" s="11" t="n"/>
+      <c r="BI8" s="11" t="n"/>
       <c r="BJ8" s="8" t="n"/>
-      <c r="BK8" s="10" t="n"/>
-      <c r="BL8" s="10" t="n"/>
-      <c r="BM8" s="10" t="n"/>
+      <c r="BK8" s="11" t="n"/>
+      <c r="BL8" s="11" t="n"/>
+      <c r="BM8" s="11" t="n"/>
       <c r="BN8" s="8" t="n"/>
-      <c r="BO8" s="10" t="n"/>
-      <c r="BP8" s="10" t="n"/>
-      <c r="BQ8" s="10" t="n"/>
+      <c r="BO8" s="11" t="n"/>
+      <c r="BP8" s="11" t="n"/>
+      <c r="BQ8" s="11" t="n"/>
       <c r="BR8" s="7" t="n"/>
     </row>
     <row r="9">
@@ -1321,17 +1330,17 @@
         </is>
       </c>
       <c r="D11" s="8" t="n"/>
-      <c r="E11" s="10" t="n"/>
-      <c r="F11" s="10" t="n"/>
-      <c r="G11" s="10" t="n"/>
+      <c r="E11" s="11" t="n"/>
+      <c r="F11" s="11" t="n"/>
+      <c r="G11" s="11" t="n"/>
       <c r="H11" s="8" t="n"/>
-      <c r="I11" s="10" t="n"/>
-      <c r="J11" s="10" t="n"/>
-      <c r="K11" s="10" t="n"/>
+      <c r="I11" s="11" t="n"/>
+      <c r="J11" s="11" t="n"/>
+      <c r="K11" s="11" t="n"/>
       <c r="L11" s="8" t="n"/>
-      <c r="M11" s="10" t="n"/>
-      <c r="N11" s="10" t="n"/>
-      <c r="O11" s="10" t="n"/>
+      <c r="M11" s="11" t="n"/>
+      <c r="N11" s="11" t="n"/>
+      <c r="O11" s="11" t="n"/>
       <c r="P11" s="7" t="n"/>
       <c r="T11" s="4" t="n"/>
       <c r="U11" s="10" t="inlineStr">
@@ -1340,17 +1349,17 @@
         </is>
       </c>
       <c r="V11" s="8" t="n"/>
-      <c r="W11" s="10" t="n"/>
-      <c r="X11" s="10" t="n"/>
-      <c r="Y11" s="10" t="n"/>
+      <c r="W11" s="11" t="n"/>
+      <c r="X11" s="11" t="n"/>
+      <c r="Y11" s="11" t="n"/>
       <c r="Z11" s="8" t="n"/>
-      <c r="AA11" s="10" t="n"/>
-      <c r="AB11" s="10" t="n"/>
-      <c r="AC11" s="10" t="n"/>
+      <c r="AA11" s="11" t="n"/>
+      <c r="AB11" s="11" t="n"/>
+      <c r="AC11" s="11" t="n"/>
       <c r="AD11" s="8" t="n"/>
-      <c r="AE11" s="10" t="n"/>
-      <c r="AF11" s="10" t="n"/>
-      <c r="AG11" s="10" t="n"/>
+      <c r="AE11" s="11" t="n"/>
+      <c r="AF11" s="11" t="n"/>
+      <c r="AG11" s="11" t="n"/>
       <c r="AH11" s="7" t="n"/>
       <c r="AL11" s="4" t="n"/>
       <c r="AM11" s="10" t="inlineStr">
@@ -1359,17 +1368,17 @@
         </is>
       </c>
       <c r="AN11" s="8" t="n"/>
-      <c r="AO11" s="10" t="n"/>
-      <c r="AP11" s="10" t="n"/>
-      <c r="AQ11" s="10" t="n"/>
+      <c r="AO11" s="11" t="n"/>
+      <c r="AP11" s="11" t="n"/>
+      <c r="AQ11" s="11" t="n"/>
       <c r="AR11" s="8" t="n"/>
-      <c r="AS11" s="10" t="n"/>
-      <c r="AT11" s="10" t="n"/>
-      <c r="AU11" s="10" t="n"/>
+      <c r="AS11" s="11" t="n"/>
+      <c r="AT11" s="11" t="n"/>
+      <c r="AU11" s="11" t="n"/>
       <c r="AV11" s="8" t="n"/>
-      <c r="AW11" s="10" t="n"/>
-      <c r="AX11" s="10" t="n"/>
-      <c r="AY11" s="10" t="n"/>
+      <c r="AW11" s="11" t="n"/>
+      <c r="AX11" s="11" t="n"/>
+      <c r="AY11" s="11" t="n"/>
       <c r="AZ11" s="7" t="n"/>
       <c r="BD11" s="4" t="n"/>
       <c r="BE11" s="10" t="inlineStr">
@@ -1378,17 +1387,17 @@
         </is>
       </c>
       <c r="BF11" s="8" t="n"/>
-      <c r="BG11" s="10" t="n"/>
-      <c r="BH11" s="10" t="n"/>
-      <c r="BI11" s="10" t="n"/>
+      <c r="BG11" s="11" t="n"/>
+      <c r="BH11" s="11" t="n"/>
+      <c r="BI11" s="11" t="n"/>
       <c r="BJ11" s="8" t="n"/>
-      <c r="BK11" s="10" t="n"/>
-      <c r="BL11" s="10" t="n"/>
-      <c r="BM11" s="10" t="n"/>
+      <c r="BK11" s="11" t="n"/>
+      <c r="BL11" s="11" t="n"/>
+      <c r="BM11" s="11" t="n"/>
       <c r="BN11" s="8" t="n"/>
-      <c r="BO11" s="10" t="n"/>
-      <c r="BP11" s="10" t="n"/>
-      <c r="BQ11" s="10" t="n"/>
+      <c r="BO11" s="11" t="n"/>
+      <c r="BP11" s="11" t="n"/>
+      <c r="BQ11" s="11" t="n"/>
       <c r="BR11" s="7" t="n"/>
     </row>
     <row r="12">
@@ -1523,17 +1532,17 @@
         </is>
       </c>
       <c r="D14" s="8" t="n"/>
-      <c r="E14" s="10" t="n"/>
-      <c r="F14" s="10" t="n"/>
-      <c r="G14" s="10" t="n"/>
+      <c r="E14" s="11" t="n"/>
+      <c r="F14" s="11" t="n"/>
+      <c r="G14" s="11" t="n"/>
       <c r="H14" s="8" t="n"/>
-      <c r="I14" s="10" t="n"/>
-      <c r="J14" s="10" t="n"/>
-      <c r="K14" s="10" t="n"/>
+      <c r="I14" s="11" t="n"/>
+      <c r="J14" s="11" t="n"/>
+      <c r="K14" s="11" t="n"/>
       <c r="L14" s="8" t="n"/>
-      <c r="M14" s="10" t="n"/>
-      <c r="N14" s="10" t="n"/>
-      <c r="O14" s="10" t="n"/>
+      <c r="M14" s="11" t="n"/>
+      <c r="N14" s="11" t="n"/>
+      <c r="O14" s="11" t="n"/>
       <c r="P14" s="7" t="n"/>
       <c r="T14" s="4" t="n"/>
       <c r="U14" s="10" t="inlineStr">
@@ -1542,17 +1551,17 @@
         </is>
       </c>
       <c r="V14" s="8" t="n"/>
-      <c r="W14" s="10" t="n"/>
-      <c r="X14" s="10" t="n"/>
-      <c r="Y14" s="10" t="n"/>
+      <c r="W14" s="11" t="n"/>
+      <c r="X14" s="11" t="n"/>
+      <c r="Y14" s="11" t="n"/>
       <c r="Z14" s="8" t="n"/>
-      <c r="AA14" s="10" t="n"/>
-      <c r="AB14" s="10" t="n"/>
-      <c r="AC14" s="10" t="n"/>
+      <c r="AA14" s="11" t="n"/>
+      <c r="AB14" s="11" t="n"/>
+      <c r="AC14" s="11" t="n"/>
       <c r="AD14" s="8" t="n"/>
-      <c r="AE14" s="10" t="n"/>
-      <c r="AF14" s="10" t="n"/>
-      <c r="AG14" s="10" t="n"/>
+      <c r="AE14" s="11" t="n"/>
+      <c r="AF14" s="11" t="n"/>
+      <c r="AG14" s="11" t="n"/>
       <c r="AH14" s="7" t="n"/>
       <c r="AL14" s="4" t="n"/>
       <c r="AM14" s="10" t="inlineStr">
@@ -1561,17 +1570,17 @@
         </is>
       </c>
       <c r="AN14" s="8" t="n"/>
-      <c r="AO14" s="10" t="n"/>
-      <c r="AP14" s="10" t="n"/>
-      <c r="AQ14" s="10" t="n"/>
+      <c r="AO14" s="11" t="n"/>
+      <c r="AP14" s="11" t="n"/>
+      <c r="AQ14" s="11" t="n"/>
       <c r="AR14" s="8" t="n"/>
-      <c r="AS14" s="10" t="n"/>
-      <c r="AT14" s="10" t="n"/>
-      <c r="AU14" s="10" t="n"/>
+      <c r="AS14" s="11" t="n"/>
+      <c r="AT14" s="11" t="n"/>
+      <c r="AU14" s="11" t="n"/>
       <c r="AV14" s="8" t="n"/>
-      <c r="AW14" s="10" t="n"/>
-      <c r="AX14" s="10" t="n"/>
-      <c r="AY14" s="10" t="n"/>
+      <c r="AW14" s="11" t="n"/>
+      <c r="AX14" s="11" t="n"/>
+      <c r="AY14" s="11" t="n"/>
       <c r="AZ14" s="7" t="n"/>
       <c r="BD14" s="4" t="n"/>
       <c r="BE14" s="10" t="inlineStr">
@@ -1580,17 +1589,17 @@
         </is>
       </c>
       <c r="BF14" s="8" t="n"/>
-      <c r="BG14" s="10" t="n"/>
-      <c r="BH14" s="10" t="n"/>
-      <c r="BI14" s="10" t="n"/>
+      <c r="BG14" s="11" t="n"/>
+      <c r="BH14" s="11" t="n"/>
+      <c r="BI14" s="11" t="n"/>
       <c r="BJ14" s="8" t="n"/>
-      <c r="BK14" s="10" t="n"/>
-      <c r="BL14" s="10" t="n"/>
-      <c r="BM14" s="10" t="n"/>
+      <c r="BK14" s="11" t="n"/>
+      <c r="BL14" s="11" t="n"/>
+      <c r="BM14" s="11" t="n"/>
       <c r="BN14" s="8" t="n"/>
-      <c r="BO14" s="10" t="n"/>
-      <c r="BP14" s="10" t="n"/>
-      <c r="BQ14" s="10" t="n"/>
+      <c r="BO14" s="11" t="n"/>
+      <c r="BP14" s="11" t="n"/>
+      <c r="BQ14" s="11" t="n"/>
       <c r="BR14" s="7" t="n"/>
     </row>
     <row r="15">
@@ -1725,17 +1734,17 @@
         </is>
       </c>
       <c r="D17" s="8" t="n"/>
-      <c r="E17" s="10" t="n"/>
-      <c r="F17" s="10" t="n"/>
-      <c r="G17" s="10" t="n"/>
+      <c r="E17" s="11" t="n"/>
+      <c r="F17" s="11" t="n"/>
+      <c r="G17" s="11" t="n"/>
       <c r="H17" s="8" t="n"/>
-      <c r="I17" s="10" t="n"/>
-      <c r="J17" s="10" t="n"/>
-      <c r="K17" s="10" t="n"/>
+      <c r="I17" s="11" t="n"/>
+      <c r="J17" s="11" t="n"/>
+      <c r="K17" s="11" t="n"/>
       <c r="L17" s="8" t="n"/>
-      <c r="M17" s="10" t="n"/>
-      <c r="N17" s="10" t="n"/>
-      <c r="O17" s="10" t="n"/>
+      <c r="M17" s="11" t="n"/>
+      <c r="N17" s="11" t="n"/>
+      <c r="O17" s="11" t="n"/>
       <c r="P17" s="7" t="n"/>
       <c r="T17" s="4" t="n"/>
       <c r="U17" s="10" t="inlineStr">
@@ -1744,17 +1753,17 @@
         </is>
       </c>
       <c r="V17" s="8" t="n"/>
-      <c r="W17" s="10" t="n"/>
-      <c r="X17" s="10" t="n"/>
-      <c r="Y17" s="10" t="n"/>
+      <c r="W17" s="11" t="n"/>
+      <c r="X17" s="11" t="n"/>
+      <c r="Y17" s="11" t="n"/>
       <c r="Z17" s="8" t="n"/>
-      <c r="AA17" s="10" t="n"/>
-      <c r="AB17" s="10" t="n"/>
-      <c r="AC17" s="10" t="n"/>
+      <c r="AA17" s="11" t="n"/>
+      <c r="AB17" s="11" t="n"/>
+      <c r="AC17" s="11" t="n"/>
       <c r="AD17" s="8" t="n"/>
-      <c r="AE17" s="10" t="n"/>
-      <c r="AF17" s="10" t="n"/>
-      <c r="AG17" s="10" t="n"/>
+      <c r="AE17" s="11" t="n"/>
+      <c r="AF17" s="11" t="n"/>
+      <c r="AG17" s="11" t="n"/>
       <c r="AH17" s="7" t="n"/>
       <c r="AL17" s="4" t="n"/>
       <c r="AM17" s="10" t="inlineStr">
@@ -1763,17 +1772,17 @@
         </is>
       </c>
       <c r="AN17" s="8" t="n"/>
-      <c r="AO17" s="10" t="n"/>
-      <c r="AP17" s="10" t="n"/>
-      <c r="AQ17" s="10" t="n"/>
+      <c r="AO17" s="11" t="n"/>
+      <c r="AP17" s="11" t="n"/>
+      <c r="AQ17" s="11" t="n"/>
       <c r="AR17" s="8" t="n"/>
-      <c r="AS17" s="10" t="n"/>
-      <c r="AT17" s="10" t="n"/>
-      <c r="AU17" s="10" t="n"/>
+      <c r="AS17" s="11" t="n"/>
+      <c r="AT17" s="11" t="n"/>
+      <c r="AU17" s="11" t="n"/>
       <c r="AV17" s="8" t="n"/>
-      <c r="AW17" s="10" t="n"/>
-      <c r="AX17" s="10" t="n"/>
-      <c r="AY17" s="10" t="n"/>
+      <c r="AW17" s="11" t="n"/>
+      <c r="AX17" s="11" t="n"/>
+      <c r="AY17" s="11" t="n"/>
       <c r="AZ17" s="7" t="n"/>
       <c r="BD17" s="4" t="n"/>
       <c r="BE17" s="10" t="inlineStr">
@@ -1782,17 +1791,17 @@
         </is>
       </c>
       <c r="BF17" s="8" t="n"/>
-      <c r="BG17" s="10" t="n"/>
-      <c r="BH17" s="10" t="n"/>
-      <c r="BI17" s="10" t="n"/>
+      <c r="BG17" s="11" t="n"/>
+      <c r="BH17" s="11" t="n"/>
+      <c r="BI17" s="11" t="n"/>
       <c r="BJ17" s="8" t="n"/>
-      <c r="BK17" s="10" t="n"/>
-      <c r="BL17" s="10" t="n"/>
-      <c r="BM17" s="10" t="n"/>
+      <c r="BK17" s="11" t="n"/>
+      <c r="BL17" s="11" t="n"/>
+      <c r="BM17" s="11" t="n"/>
       <c r="BN17" s="8" t="n"/>
-      <c r="BO17" s="10" t="n"/>
-      <c r="BP17" s="10" t="n"/>
-      <c r="BQ17" s="10" t="n"/>
+      <c r="BO17" s="11" t="n"/>
+      <c r="BP17" s="11" t="n"/>
+      <c r="BQ17" s="11" t="n"/>
       <c r="BR17" s="7" t="n"/>
     </row>
     <row r="18">
@@ -1927,17 +1936,17 @@
         </is>
       </c>
       <c r="D20" s="8" t="n"/>
-      <c r="E20" s="10" t="n"/>
-      <c r="F20" s="10" t="n"/>
-      <c r="G20" s="10" t="n"/>
+      <c r="E20" s="11" t="n"/>
+      <c r="F20" s="11" t="n"/>
+      <c r="G20" s="11" t="n"/>
       <c r="H20" s="8" t="n"/>
-      <c r="I20" s="10" t="n"/>
-      <c r="J20" s="10" t="n"/>
-      <c r="K20" s="10" t="n"/>
+      <c r="I20" s="11" t="n"/>
+      <c r="J20" s="11" t="n"/>
+      <c r="K20" s="11" t="n"/>
       <c r="L20" s="8" t="n"/>
-      <c r="M20" s="10" t="n"/>
-      <c r="N20" s="10" t="n"/>
-      <c r="O20" s="10" t="n"/>
+      <c r="M20" s="11" t="n"/>
+      <c r="N20" s="11" t="n"/>
+      <c r="O20" s="11" t="n"/>
       <c r="P20" s="7" t="n"/>
       <c r="T20" s="4" t="n"/>
       <c r="U20" s="10" t="inlineStr">
@@ -1946,17 +1955,17 @@
         </is>
       </c>
       <c r="V20" s="8" t="n"/>
-      <c r="W20" s="10" t="n"/>
-      <c r="X20" s="10" t="n"/>
-      <c r="Y20" s="10" t="n"/>
+      <c r="W20" s="11" t="n"/>
+      <c r="X20" s="11" t="n"/>
+      <c r="Y20" s="11" t="n"/>
       <c r="Z20" s="8" t="n"/>
-      <c r="AA20" s="10" t="n"/>
-      <c r="AB20" s="10" t="n"/>
-      <c r="AC20" s="10" t="n"/>
+      <c r="AA20" s="11" t="n"/>
+      <c r="AB20" s="11" t="n"/>
+      <c r="AC20" s="11" t="n"/>
       <c r="AD20" s="8" t="n"/>
-      <c r="AE20" s="10" t="n"/>
-      <c r="AF20" s="10" t="n"/>
-      <c r="AG20" s="10" t="n"/>
+      <c r="AE20" s="11" t="n"/>
+      <c r="AF20" s="11" t="n"/>
+      <c r="AG20" s="11" t="n"/>
       <c r="AH20" s="7" t="n"/>
       <c r="AL20" s="4" t="n"/>
       <c r="AM20" s="10" t="inlineStr">
@@ -1965,17 +1974,17 @@
         </is>
       </c>
       <c r="AN20" s="8" t="n"/>
-      <c r="AO20" s="10" t="n"/>
-      <c r="AP20" s="10" t="n"/>
-      <c r="AQ20" s="10" t="n"/>
+      <c r="AO20" s="11" t="n"/>
+      <c r="AP20" s="11" t="n"/>
+      <c r="AQ20" s="11" t="n"/>
       <c r="AR20" s="8" t="n"/>
-      <c r="AS20" s="10" t="n"/>
-      <c r="AT20" s="10" t="n"/>
-      <c r="AU20" s="10" t="n"/>
+      <c r="AS20" s="11" t="n"/>
+      <c r="AT20" s="11" t="n"/>
+      <c r="AU20" s="11" t="n"/>
       <c r="AV20" s="8" t="n"/>
-      <c r="AW20" s="10" t="n"/>
-      <c r="AX20" s="10" t="n"/>
-      <c r="AY20" s="10" t="n"/>
+      <c r="AW20" s="11" t="n"/>
+      <c r="AX20" s="11" t="n"/>
+      <c r="AY20" s="11" t="n"/>
       <c r="AZ20" s="7" t="n"/>
       <c r="BD20" s="4" t="n"/>
       <c r="BE20" s="10" t="inlineStr">
@@ -1984,17 +1993,17 @@
         </is>
       </c>
       <c r="BF20" s="8" t="n"/>
-      <c r="BG20" s="10" t="n"/>
-      <c r="BH20" s="10" t="n"/>
-      <c r="BI20" s="10" t="n"/>
+      <c r="BG20" s="11" t="n"/>
+      <c r="BH20" s="11" t="n"/>
+      <c r="BI20" s="11" t="n"/>
       <c r="BJ20" s="8" t="n"/>
-      <c r="BK20" s="10" t="n"/>
-      <c r="BL20" s="10" t="n"/>
-      <c r="BM20" s="10" t="n"/>
+      <c r="BK20" s="11" t="n"/>
+      <c r="BL20" s="11" t="n"/>
+      <c r="BM20" s="11" t="n"/>
       <c r="BN20" s="8" t="n"/>
-      <c r="BO20" s="10" t="n"/>
-      <c r="BP20" s="10" t="n"/>
-      <c r="BQ20" s="10" t="n"/>
+      <c r="BO20" s="11" t="n"/>
+      <c r="BP20" s="11" t="n"/>
+      <c r="BQ20" s="11" t="n"/>
       <c r="BR20" s="7" t="n"/>
     </row>
     <row r="21">
@@ -2129,17 +2138,17 @@
         </is>
       </c>
       <c r="D23" s="8" t="n"/>
-      <c r="E23" s="10" t="n"/>
-      <c r="F23" s="10" t="n"/>
-      <c r="G23" s="10" t="n"/>
+      <c r="E23" s="11" t="n"/>
+      <c r="F23" s="11" t="n"/>
+      <c r="G23" s="11" t="n"/>
       <c r="H23" s="8" t="n"/>
-      <c r="I23" s="10" t="n"/>
-      <c r="J23" s="10" t="n"/>
-      <c r="K23" s="10" t="n"/>
+      <c r="I23" s="11" t="n"/>
+      <c r="J23" s="11" t="n"/>
+      <c r="K23" s="11" t="n"/>
       <c r="L23" s="8" t="n"/>
-      <c r="M23" s="10" t="n"/>
-      <c r="N23" s="10" t="n"/>
-      <c r="O23" s="10" t="n"/>
+      <c r="M23" s="11" t="n"/>
+      <c r="N23" s="11" t="n"/>
+      <c r="O23" s="11" t="n"/>
       <c r="P23" s="7" t="n"/>
       <c r="T23" s="4" t="n"/>
       <c r="U23" s="10" t="inlineStr">
@@ -2148,17 +2157,17 @@
         </is>
       </c>
       <c r="V23" s="8" t="n"/>
-      <c r="W23" s="10" t="n"/>
-      <c r="X23" s="10" t="n"/>
-      <c r="Y23" s="10" t="n"/>
+      <c r="W23" s="11" t="n"/>
+      <c r="X23" s="11" t="n"/>
+      <c r="Y23" s="11" t="n"/>
       <c r="Z23" s="8" t="n"/>
-      <c r="AA23" s="10" t="n"/>
-      <c r="AB23" s="10" t="n"/>
-      <c r="AC23" s="10" t="n"/>
+      <c r="AA23" s="11" t="n"/>
+      <c r="AB23" s="11" t="n"/>
+      <c r="AC23" s="11" t="n"/>
       <c r="AD23" s="8" t="n"/>
-      <c r="AE23" s="10" t="n"/>
-      <c r="AF23" s="10" t="n"/>
-      <c r="AG23" s="10" t="n"/>
+      <c r="AE23" s="11" t="n"/>
+      <c r="AF23" s="11" t="n"/>
+      <c r="AG23" s="11" t="n"/>
       <c r="AH23" s="7" t="n"/>
       <c r="AL23" s="4" t="n"/>
       <c r="AM23" s="10" t="inlineStr">
@@ -2167,17 +2176,17 @@
         </is>
       </c>
       <c r="AN23" s="8" t="n"/>
-      <c r="AO23" s="10" t="n"/>
-      <c r="AP23" s="10" t="n"/>
-      <c r="AQ23" s="10" t="n"/>
+      <c r="AO23" s="11" t="n"/>
+      <c r="AP23" s="11" t="n"/>
+      <c r="AQ23" s="11" t="n"/>
       <c r="AR23" s="8" t="n"/>
-      <c r="AS23" s="10" t="n"/>
-      <c r="AT23" s="10" t="n"/>
-      <c r="AU23" s="10" t="n"/>
+      <c r="AS23" s="11" t="n"/>
+      <c r="AT23" s="11" t="n"/>
+      <c r="AU23" s="11" t="n"/>
       <c r="AV23" s="8" t="n"/>
-      <c r="AW23" s="10" t="n"/>
-      <c r="AX23" s="10" t="n"/>
-      <c r="AY23" s="10" t="n"/>
+      <c r="AW23" s="11" t="n"/>
+      <c r="AX23" s="11" t="n"/>
+      <c r="AY23" s="11" t="n"/>
       <c r="AZ23" s="7" t="n"/>
       <c r="BD23" s="4" t="n"/>
       <c r="BE23" s="10" t="inlineStr">
@@ -2186,17 +2195,17 @@
         </is>
       </c>
       <c r="BF23" s="8" t="n"/>
-      <c r="BG23" s="10" t="n"/>
-      <c r="BH23" s="10" t="n"/>
-      <c r="BI23" s="10" t="n"/>
+      <c r="BG23" s="11" t="n"/>
+      <c r="BH23" s="11" t="n"/>
+      <c r="BI23" s="11" t="n"/>
       <c r="BJ23" s="8" t="n"/>
-      <c r="BK23" s="10" t="n"/>
-      <c r="BL23" s="10" t="n"/>
-      <c r="BM23" s="10" t="n"/>
+      <c r="BK23" s="11" t="n"/>
+      <c r="BL23" s="11" t="n"/>
+      <c r="BM23" s="11" t="n"/>
       <c r="BN23" s="8" t="n"/>
-      <c r="BO23" s="10" t="n"/>
-      <c r="BP23" s="10" t="n"/>
-      <c r="BQ23" s="10" t="n"/>
+      <c r="BO23" s="11" t="n"/>
+      <c r="BP23" s="11" t="n"/>
+      <c r="BQ23" s="11" t="n"/>
       <c r="BR23" s="7" t="n"/>
     </row>
     <row r="24">
@@ -2331,17 +2340,17 @@
         </is>
       </c>
       <c r="D26" s="8" t="n"/>
-      <c r="E26" s="10" t="n"/>
-      <c r="F26" s="10" t="n"/>
-      <c r="G26" s="10" t="n"/>
+      <c r="E26" s="11" t="n"/>
+      <c r="F26" s="11" t="n"/>
+      <c r="G26" s="11" t="n"/>
       <c r="H26" s="8" t="n"/>
-      <c r="I26" s="10" t="n"/>
-      <c r="J26" s="10" t="n"/>
-      <c r="K26" s="10" t="n"/>
+      <c r="I26" s="11" t="n"/>
+      <c r="J26" s="11" t="n"/>
+      <c r="K26" s="11" t="n"/>
       <c r="L26" s="8" t="n"/>
-      <c r="M26" s="10" t="n"/>
-      <c r="N26" s="10" t="n"/>
-      <c r="O26" s="10" t="n"/>
+      <c r="M26" s="11" t="n"/>
+      <c r="N26" s="11" t="n"/>
+      <c r="O26" s="11" t="n"/>
       <c r="P26" s="7" t="n"/>
       <c r="T26" s="4" t="n"/>
       <c r="U26" s="10" t="inlineStr">
@@ -2350,17 +2359,17 @@
         </is>
       </c>
       <c r="V26" s="8" t="n"/>
-      <c r="W26" s="10" t="n"/>
-      <c r="X26" s="10" t="n"/>
-      <c r="Y26" s="10" t="n"/>
+      <c r="W26" s="11" t="n"/>
+      <c r="X26" s="11" t="n"/>
+      <c r="Y26" s="11" t="n"/>
       <c r="Z26" s="8" t="n"/>
-      <c r="AA26" s="10" t="n"/>
-      <c r="AB26" s="10" t="n"/>
-      <c r="AC26" s="10" t="n"/>
+      <c r="AA26" s="11" t="n"/>
+      <c r="AB26" s="11" t="n"/>
+      <c r="AC26" s="11" t="n"/>
       <c r="AD26" s="8" t="n"/>
-      <c r="AE26" s="10" t="n"/>
-      <c r="AF26" s="10" t="n"/>
-      <c r="AG26" s="10" t="n"/>
+      <c r="AE26" s="11" t="n"/>
+      <c r="AF26" s="11" t="n"/>
+      <c r="AG26" s="11" t="n"/>
       <c r="AH26" s="7" t="n"/>
       <c r="AL26" s="4" t="n"/>
       <c r="AM26" s="10" t="inlineStr">
@@ -2369,17 +2378,17 @@
         </is>
       </c>
       <c r="AN26" s="8" t="n"/>
-      <c r="AO26" s="10" t="n"/>
-      <c r="AP26" s="10" t="n"/>
-      <c r="AQ26" s="10" t="n"/>
+      <c r="AO26" s="11" t="n"/>
+      <c r="AP26" s="11" t="n"/>
+      <c r="AQ26" s="11" t="n"/>
       <c r="AR26" s="8" t="n"/>
-      <c r="AS26" s="10" t="n"/>
-      <c r="AT26" s="10" t="n"/>
-      <c r="AU26" s="10" t="n"/>
+      <c r="AS26" s="11" t="n"/>
+      <c r="AT26" s="11" t="n"/>
+      <c r="AU26" s="11" t="n"/>
       <c r="AV26" s="8" t="n"/>
-      <c r="AW26" s="10" t="n"/>
-      <c r="AX26" s="10" t="n"/>
-      <c r="AY26" s="10" t="n"/>
+      <c r="AW26" s="11" t="n"/>
+      <c r="AX26" s="11" t="n"/>
+      <c r="AY26" s="11" t="n"/>
       <c r="AZ26" s="7" t="n"/>
       <c r="BD26" s="4" t="n"/>
       <c r="BE26" s="10" t="inlineStr">
@@ -2388,17 +2397,17 @@
         </is>
       </c>
       <c r="BF26" s="8" t="n"/>
-      <c r="BG26" s="10" t="n"/>
-      <c r="BH26" s="10" t="n"/>
-      <c r="BI26" s="10" t="n"/>
+      <c r="BG26" s="11" t="n"/>
+      <c r="BH26" s="11" t="n"/>
+      <c r="BI26" s="11" t="n"/>
       <c r="BJ26" s="8" t="n"/>
-      <c r="BK26" s="10" t="n"/>
-      <c r="BL26" s="10" t="n"/>
-      <c r="BM26" s="10" t="n"/>
+      <c r="BK26" s="11" t="n"/>
+      <c r="BL26" s="11" t="n"/>
+      <c r="BM26" s="11" t="n"/>
       <c r="BN26" s="8" t="n"/>
-      <c r="BO26" s="10" t="n"/>
-      <c r="BP26" s="10" t="n"/>
-      <c r="BQ26" s="10" t="n"/>
+      <c r="BO26" s="11" t="n"/>
+      <c r="BP26" s="11" t="n"/>
+      <c r="BQ26" s="11" t="n"/>
       <c r="BR26" s="7" t="n"/>
     </row>
     <row r="27">

</xml_diff>